<commit_message>
logging and error handling
</commit_message>
<xml_diff>
--- a/stars/Stars.xlsx
+++ b/stars/Stars.xlsx
@@ -762,10 +762,8 @@
       <c r="K5" s="10" t="n">
         <v>0</v>
       </c>
-      <c r="L5" s="10" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+      <c r="L5" s="10" t="n">
+        <v>0</v>
       </c>
       <c r="M5" s="10" t="inlineStr">
         <is>
@@ -871,10 +869,8 @@
       <c r="K6" s="10" t="n">
         <v>0</v>
       </c>
-      <c r="L6" s="10" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+      <c r="L6" s="10" t="n">
+        <v>0</v>
       </c>
       <c r="M6" s="10" t="inlineStr">
         <is>
@@ -980,10 +976,8 @@
       <c r="K7" s="10" t="n">
         <v>0</v>
       </c>
-      <c r="L7" s="10" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+      <c r="L7" s="10" t="n">
+        <v>0</v>
       </c>
       <c r="M7" s="10" t="inlineStr">
         <is>
@@ -1083,11 +1077,7 @@
       <c r="I8" s="10" t="inlineStr"/>
       <c r="J8" s="10" t="inlineStr"/>
       <c r="K8" s="10" t="inlineStr"/>
-      <c r="L8" s="10" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
+      <c r="L8" s="10" t="inlineStr"/>
       <c r="M8" s="10" t="inlineStr">
         <is>
           <t>-</t>
@@ -1192,10 +1182,8 @@
       <c r="K9" s="10" t="n">
         <v>0</v>
       </c>
-      <c r="L9" s="10" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+      <c r="L9" s="10" t="n">
+        <v>0</v>
       </c>
       <c r="M9" s="10" t="inlineStr">
         <is>
@@ -1301,10 +1289,8 @@
       <c r="K10" s="10" t="n">
         <v>0</v>
       </c>
-      <c r="L10" s="10" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+      <c r="L10" s="10" t="n">
+        <v>0</v>
       </c>
       <c r="M10" s="10" t="inlineStr">
         <is>
@@ -1404,11 +1390,7 @@
       <c r="I11" s="10" t="inlineStr"/>
       <c r="J11" s="10" t="inlineStr"/>
       <c r="K11" s="10" t="inlineStr"/>
-      <c r="L11" s="10" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
+      <c r="L11" s="10" t="inlineStr"/>
       <c r="M11" s="10" t="inlineStr">
         <is>
           <t>-</t>
@@ -1513,10 +1495,8 @@
       <c r="K12" s="10" t="n">
         <v>0</v>
       </c>
-      <c r="L12" s="10" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+      <c r="L12" s="10" t="n">
+        <v>0</v>
       </c>
       <c r="M12" s="10" t="inlineStr">
         <is>

</xml_diff>